<commit_message>
added more plots, and export csv
</commit_message>
<xml_diff>
--- a/sensitivity_analysis/sensitivity_analysis_parameters.xlsx
+++ b/sensitivity_analysis/sensitivity_analysis_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSCode_python\4th_gen_dh\sensitivity_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucacasamassima/Programming/4th_gen_dh/sensitivity_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4693C2B1-0B64-44C8-B248-636E3270A4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAA3AB1-3A20-1141-8623-87D26AF07DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="50880" windowHeight="27980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>n_steps</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>analysis_type</t>
+  </si>
+  <si>
+    <t>reduction_factor</t>
   </si>
 </sst>
 </file>
@@ -378,19 +381,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -407,7 +410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -424,7 +427,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -441,7 +444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -458,7 +461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -475,7 +478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -492,7 +495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -509,7 +512,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -523,6 +526,23 @@
         <v>0.5</v>
       </c>
       <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+      <c r="E9">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added residual value of the grid and extended its lifetime for LCOH calculation
</commit_message>
<xml_diff>
--- a/sensitivity_analysis/sensitivity_analysis_parameters.xlsx
+++ b/sensitivity_analysis/sensitivity_analysis_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucacasamassima/Programming/4th_gen_dh/sensitivity_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAA3AB1-3A20-1141-8623-87D26AF07DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7254376-7A58-7B49-9143-CE88021B5921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="50880" windowHeight="27980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -384,7 +384,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -540,7 +540,7 @@
         <v>20</v>
       </c>
       <c r="D9">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="E9">
         <v>2</v>

</xml_diff>

<commit_message>
revert everything to when I modified the LCOH exponent
</commit_message>
<xml_diff>
--- a/sensitivity_analysis/sensitivity_analysis_parameters.xlsx
+++ b/sensitivity_analysis/sensitivity_analysis_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucacasamassima/Programming/4th_gen_dh/sensitivity_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7254376-7A58-7B49-9143-CE88021B5921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAA3AB1-3A20-1141-8623-87D26AF07DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="50880" windowHeight="27980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -384,7 +384,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -540,7 +540,7 @@
         <v>20</v>
       </c>
       <c r="D9">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E9">
         <v>2</v>

</xml_diff>